<commit_message>
analisa HM setiap cabang
</commit_message>
<xml_diff>
--- a/Laporan_BBM_Revisi_Final8.xlsx
+++ b/Laporan_BBM_Revisi_Final8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Downloads\SPIL\bbm\Analisa BBM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47904E7D-3A1A-4EFC-9895-DD3E495E82A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00368821-2759-4E39-8EB6-80B3C961C01F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1437,7 +1437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1445,7 +1445,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1749,12 +1748,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AKT300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A234" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A252" activeCellId="7" sqref="A237 A235 A228:A232 A241:A242 A244 A246:A247 A250 A252"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E246" sqref="E246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1763,9 +1761,9 @@
     <col min="2" max="2" width="26.140625" customWidth="1"/>
     <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="23" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
     <col min="8" max="8" width="22.28515625" customWidth="1"/>
     <col min="9" max="9" width="22.140625" customWidth="1"/>
     <col min="10" max="10" width="20.85546875" customWidth="1"/>
@@ -1806,7 +1804,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>431</v>
       </c>
@@ -1841,7 +1839,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>435</v>
       </c>
@@ -1876,7 +1874,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>431</v>
       </c>
@@ -1911,7 +1909,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>437</v>
       </c>
@@ -1946,7 +1944,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>407</v>
       </c>
@@ -1981,7 +1979,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>407</v>
       </c>
@@ -2016,7 +2014,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>407</v>
       </c>
@@ -2051,7 +2049,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>407</v>
       </c>
@@ -2086,7 +2084,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>437</v>
       </c>
@@ -2121,7 +2119,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>407</v>
       </c>
@@ -2156,7 +2154,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>407</v>
       </c>
@@ -2191,7 +2189,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>407</v>
       </c>
@@ -2226,7 +2224,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>437</v>
       </c>
@@ -2261,7 +2259,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>407</v>
       </c>
@@ -2296,7 +2294,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>407</v>
       </c>
@@ -2331,7 +2329,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>441</v>
       </c>
@@ -2366,7 +2364,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>407</v>
       </c>
@@ -2401,7 +2399,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>407</v>
       </c>
@@ -2436,7 +2434,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>407</v>
       </c>
@@ -2471,7 +2469,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>424</v>
       </c>
@@ -2506,7 +2504,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>424</v>
       </c>
@@ -2541,7 +2539,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>424</v>
       </c>
@@ -2576,7 +2574,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>350</v>
       </c>
@@ -2611,7 +2609,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>407</v>
       </c>
@@ -2646,7 +2644,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>407</v>
       </c>
@@ -2681,7 +2679,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>424</v>
       </c>
@@ -2716,7 +2714,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>407</v>
       </c>
@@ -2751,7 +2749,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>11</v>
       </c>
@@ -2786,7 +2784,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:982" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:982" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>90</v>
       </c>
@@ -3792,7 +3790,7 @@
       <c r="AKS30"/>
       <c r="AKT30"/>
     </row>
-    <row r="31" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>90</v>
       </c>
@@ -4798,7 +4796,7 @@
       <c r="AKS31"/>
       <c r="AKT31"/>
     </row>
-    <row r="32" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>90</v>
       </c>
@@ -5804,7 +5802,7 @@
       <c r="AKS32"/>
       <c r="AKT32"/>
     </row>
-    <row r="33" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -6810,7 +6808,7 @@
       <c r="AKS33"/>
       <c r="AKT33"/>
     </row>
-    <row r="34" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>90</v>
       </c>
@@ -7816,7 +7814,7 @@
       <c r="AKS34"/>
       <c r="AKT34"/>
     </row>
-    <row r="35" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>90</v>
       </c>
@@ -8822,7 +8820,7 @@
       <c r="AKS35"/>
       <c r="AKT35"/>
     </row>
-    <row r="36" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>90</v>
       </c>
@@ -9828,7 +9826,7 @@
       <c r="AKS36"/>
       <c r="AKT36"/>
     </row>
-    <row r="37" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>90</v>
       </c>
@@ -10834,7 +10832,7 @@
       <c r="AKS37"/>
       <c r="AKT37"/>
     </row>
-    <row r="38" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>90</v>
       </c>
@@ -11840,7 +11838,7 @@
       <c r="AKS38"/>
       <c r="AKT38"/>
     </row>
-    <row r="39" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>90</v>
       </c>
@@ -12846,7 +12844,7 @@
       <c r="AKS39"/>
       <c r="AKT39"/>
     </row>
-    <row r="40" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>90</v>
       </c>
@@ -13852,7 +13850,7 @@
       <c r="AKS40"/>
       <c r="AKT40"/>
     </row>
-    <row r="41" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>90</v>
       </c>
@@ -14858,7 +14856,7 @@
       <c r="AKS41"/>
       <c r="AKT41"/>
     </row>
-    <row r="42" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>90</v>
       </c>
@@ -15864,7 +15862,7 @@
       <c r="AKS42"/>
       <c r="AKT42"/>
     </row>
-    <row r="43" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>90</v>
       </c>
@@ -16870,7 +16868,7 @@
       <c r="AKS43"/>
       <c r="AKT43"/>
     </row>
-    <row r="44" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>90</v>
       </c>
@@ -17876,7 +17874,7 @@
       <c r="AKS44"/>
       <c r="AKT44"/>
     </row>
-    <row r="45" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>90</v>
       </c>
@@ -18882,7 +18880,7 @@
       <c r="AKS45"/>
       <c r="AKT45"/>
     </row>
-    <row r="46" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>90</v>
       </c>
@@ -19888,7 +19886,7 @@
       <c r="AKS46"/>
       <c r="AKT46"/>
     </row>
-    <row r="47" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>424</v>
       </c>
@@ -20894,7 +20892,7 @@
       <c r="AKS47"/>
       <c r="AKT47"/>
     </row>
-    <row r="48" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>90</v>
       </c>
@@ -21900,7 +21898,7 @@
       <c r="AKS48"/>
       <c r="AKT48"/>
     </row>
-    <row r="49" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>90</v>
       </c>
@@ -22906,7 +22904,7 @@
       <c r="AKS49"/>
       <c r="AKT49"/>
     </row>
-    <row r="50" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>443</v>
       </c>
@@ -23912,7 +23910,7 @@
       <c r="AKS50"/>
       <c r="AKT50"/>
     </row>
-    <row r="51" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>90</v>
       </c>
@@ -24918,7 +24916,7 @@
       <c r="AKS51"/>
       <c r="AKT51"/>
     </row>
-    <row r="52" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>90</v>
       </c>
@@ -25924,7 +25922,7 @@
       <c r="AKS52"/>
       <c r="AKT52"/>
     </row>
-    <row r="53" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>90</v>
       </c>
@@ -26930,7 +26928,7 @@
       <c r="AKS53"/>
       <c r="AKT53"/>
     </row>
-    <row r="54" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>90</v>
       </c>
@@ -27936,7 +27934,7 @@
       <c r="AKS54"/>
       <c r="AKT54"/>
     </row>
-    <row r="55" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>90</v>
       </c>
@@ -28942,7 +28940,7 @@
       <c r="AKS55"/>
       <c r="AKT55"/>
     </row>
-    <row r="56" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>90</v>
       </c>
@@ -29948,7 +29946,7 @@
       <c r="AKS56"/>
       <c r="AKT56"/>
     </row>
-    <row r="57" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>90</v>
       </c>
@@ -30954,7 +30952,7 @@
       <c r="AKS57"/>
       <c r="AKT57"/>
     </row>
-    <row r="58" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>90</v>
       </c>
@@ -31960,7 +31958,7 @@
       <c r="AKS58"/>
       <c r="AKT58"/>
     </row>
-    <row r="59" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>90</v>
       </c>
@@ -32966,7 +32964,7 @@
       <c r="AKS59"/>
       <c r="AKT59"/>
     </row>
-    <row r="60" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>90</v>
       </c>
@@ -33972,7 +33970,7 @@
       <c r="AKS60"/>
       <c r="AKT60"/>
     </row>
-    <row r="61" spans="1:982" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:982" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>90</v>
       </c>
@@ -34978,7 +34976,7 @@
       <c r="AKS61"/>
       <c r="AKT61"/>
     </row>
-    <row r="62" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>90</v>
       </c>
@@ -35984,7 +35982,7 @@
       <c r="AKS62"/>
       <c r="AKT62"/>
     </row>
-    <row r="63" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>90</v>
       </c>
@@ -36990,7 +36988,7 @@
       <c r="AKS63"/>
       <c r="AKT63"/>
     </row>
-    <row r="64" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>90</v>
       </c>
@@ -37996,7 +37994,7 @@
       <c r="AKS64"/>
       <c r="AKT64"/>
     </row>
-    <row r="65" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>90</v>
       </c>
@@ -39002,7 +39000,7 @@
       <c r="AKS65"/>
       <c r="AKT65"/>
     </row>
-    <row r="66" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>90</v>
       </c>
@@ -40008,7 +40006,7 @@
       <c r="AKS66"/>
       <c r="AKT66"/>
     </row>
-    <row r="67" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>90</v>
       </c>
@@ -41014,7 +41012,7 @@
       <c r="AKS67"/>
       <c r="AKT67"/>
     </row>
-    <row r="68" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>90</v>
       </c>
@@ -42020,7 +42018,7 @@
       <c r="AKS68"/>
       <c r="AKT68"/>
     </row>
-    <row r="69" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>90</v>
       </c>
@@ -43026,7 +43024,7 @@
       <c r="AKS69"/>
       <c r="AKT69"/>
     </row>
-    <row r="70" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>90</v>
       </c>
@@ -44032,7 +44030,7 @@
       <c r="AKS70"/>
       <c r="AKT70"/>
     </row>
-    <row r="71" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>424</v>
       </c>
@@ -45038,7 +45036,7 @@
       <c r="AKS71"/>
       <c r="AKT71"/>
     </row>
-    <row r="72" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>90</v>
       </c>
@@ -46044,7 +46042,7 @@
       <c r="AKS72"/>
       <c r="AKT72"/>
     </row>
-    <row r="73" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>141</v>
       </c>
@@ -47050,7 +47048,7 @@
       <c r="AKS73"/>
       <c r="AKT73"/>
     </row>
-    <row r="74" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>90</v>
       </c>
@@ -48056,7 +48054,7 @@
       <c r="AKS74"/>
       <c r="AKT74"/>
     </row>
-    <row r="75" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>11</v>
       </c>
@@ -49062,7 +49060,7 @@
       <c r="AKS75"/>
       <c r="AKT75"/>
     </row>
-    <row r="76" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>90</v>
       </c>
@@ -50068,7 +50066,7 @@
       <c r="AKS76"/>
       <c r="AKT76"/>
     </row>
-    <row r="77" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>11</v>
       </c>
@@ -51074,7 +51072,7 @@
       <c r="AKS77"/>
       <c r="AKT77"/>
     </row>
-    <row r="78" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>141</v>
       </c>
@@ -51109,7 +51107,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>11</v>
       </c>
@@ -51144,7 +51142,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>141</v>
       </c>
@@ -51179,7 +51177,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>141</v>
       </c>
@@ -51214,7 +51212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>141</v>
       </c>
@@ -52220,7 +52218,7 @@
       <c r="AKS82"/>
       <c r="AKT82"/>
     </row>
-    <row r="83" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>11</v>
       </c>
@@ -52255,7 +52253,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>141</v>
       </c>
@@ -52290,7 +52288,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>141</v>
       </c>
@@ -52325,7 +52323,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>90</v>
       </c>
@@ -52360,7 +52358,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>11</v>
       </c>
@@ -52395,7 +52393,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>11</v>
       </c>
@@ -53401,7 +53399,7 @@
       <c r="AKS88"/>
       <c r="AKT88"/>
     </row>
-    <row r="89" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>90</v>
       </c>
@@ -53436,7 +53434,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>141</v>
       </c>
@@ -53471,7 +53469,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>141</v>
       </c>
@@ -53506,7 +53504,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>141</v>
       </c>
@@ -53541,7 +53539,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>141</v>
       </c>
@@ -53576,7 +53574,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>141</v>
       </c>
@@ -53611,7 +53609,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>141</v>
       </c>
@@ -53646,7 +53644,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>90</v>
       </c>
@@ -53681,7 +53679,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>11</v>
       </c>
@@ -53716,7 +53714,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>350</v>
       </c>
@@ -53751,7 +53749,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>141</v>
       </c>
@@ -53786,7 +53784,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>141</v>
       </c>
@@ -53821,7 +53819,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>141</v>
       </c>
@@ -53856,7 +53854,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>90</v>
       </c>
@@ -53891,7 +53889,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>141</v>
       </c>
@@ -53926,7 +53924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>90</v>
       </c>
@@ -54932,7 +54930,7 @@
       <c r="AKS104"/>
       <c r="AKT104"/>
     </row>
-    <row r="105" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>141</v>
       </c>
@@ -54967,7 +54965,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>11</v>
       </c>
@@ -55002,7 +55000,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>141</v>
       </c>
@@ -55037,7 +55035,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>350</v>
       </c>
@@ -55072,7 +55070,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>11</v>
       </c>
@@ -55107,7 +55105,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>11</v>
       </c>
@@ -55142,7 +55140,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>11</v>
       </c>
@@ -55177,7 +55175,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>350</v>
       </c>
@@ -55212,7 +55210,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>141</v>
       </c>
@@ -55247,7 +55245,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>431</v>
       </c>
@@ -55282,7 +55280,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>141</v>
       </c>
@@ -55317,7 +55315,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>11</v>
       </c>
@@ -55352,7 +55350,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>141</v>
       </c>
@@ -55387,7 +55385,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>11</v>
       </c>
@@ -56393,7 +56391,7 @@
       <c r="AKS118"/>
       <c r="AKT118"/>
     </row>
-    <row r="119" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>350</v>
       </c>
@@ -56428,7 +56426,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>141</v>
       </c>
@@ -56463,7 +56461,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>141</v>
       </c>
@@ -56498,7 +56496,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>141</v>
       </c>
@@ -56533,7 +56531,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>141</v>
       </c>
@@ -56568,7 +56566,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>141</v>
       </c>
@@ -56603,7 +56601,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>141</v>
       </c>
@@ -56638,7 +56636,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>141</v>
       </c>
@@ -56673,7 +56671,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>350</v>
       </c>
@@ -56708,7 +56706,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>141</v>
       </c>
@@ -56743,7 +56741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>141</v>
       </c>
@@ -57749,7 +57747,7 @@
       <c r="AKS129"/>
       <c r="AKT129"/>
     </row>
-    <row r="130" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>141</v>
       </c>
@@ -57784,7 +57782,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>141</v>
       </c>
@@ -57819,7 +57817,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="132" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>11</v>
       </c>
@@ -57854,7 +57852,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="133" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>11</v>
       </c>
@@ -57889,7 +57887,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>141</v>
       </c>
@@ -57924,7 +57922,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="135" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>11</v>
       </c>
@@ -57959,7 +57957,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="136" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>11</v>
       </c>
@@ -57994,7 +57992,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="137" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>141</v>
       </c>
@@ -58029,7 +58027,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="138" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>141</v>
       </c>
@@ -58064,7 +58062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="139" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>141</v>
       </c>
@@ -58099,7 +58097,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="140" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>141</v>
       </c>
@@ -58134,7 +58132,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="141" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>141</v>
       </c>
@@ -58169,7 +58167,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="142" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>141</v>
       </c>
@@ -58204,7 +58202,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="143" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>11</v>
       </c>
@@ -58239,7 +58237,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="144" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>141</v>
       </c>
@@ -58274,7 +58272,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="145" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>141</v>
       </c>
@@ -58309,7 +58307,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="146" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>141</v>
       </c>
@@ -58344,7 +58342,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="147" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>141</v>
       </c>
@@ -58379,7 +58377,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="148" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>141</v>
       </c>
@@ -58414,7 +58412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="149" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>141</v>
       </c>
@@ -58449,7 +58447,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="150" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>11</v>
       </c>
@@ -58484,7 +58482,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="151" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>11</v>
       </c>
@@ -58519,7 +58517,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="152" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>141</v>
       </c>
@@ -58554,7 +58552,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>141</v>
       </c>
@@ -58589,7 +58587,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>141</v>
       </c>
@@ -58624,7 +58622,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>141</v>
       </c>
@@ -58659,7 +58657,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>141</v>
       </c>
@@ -58694,7 +58692,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="157" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>141</v>
       </c>
@@ -59700,7 +59698,7 @@
       <c r="AKS157"/>
       <c r="AKT157"/>
     </row>
-    <row r="158" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>11</v>
       </c>
@@ -59735,7 +59733,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="159" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>141</v>
       </c>
@@ -59770,7 +59768,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="160" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>141</v>
       </c>
@@ -59805,7 +59803,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>141</v>
       </c>
@@ -59840,7 +59838,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="162" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>141</v>
       </c>
@@ -59875,7 +59873,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="163" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>141</v>
       </c>
@@ -59910,7 +59908,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="164" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>11</v>
       </c>
@@ -59945,7 +59943,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="165" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>350</v>
       </c>
@@ -59980,7 +59978,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>11</v>
       </c>
@@ -60015,7 +60013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>11</v>
       </c>
@@ -60050,7 +60048,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="168" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>11</v>
       </c>
@@ -60085,7 +60083,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="169" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>141</v>
       </c>
@@ -60120,7 +60118,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="170" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>350</v>
       </c>
@@ -60155,7 +60153,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="171" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>11</v>
       </c>
@@ -60190,7 +60188,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="172" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>11</v>
       </c>
@@ -60225,7 +60223,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="173" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>11</v>
       </c>
@@ -60260,7 +60258,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="174" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>141</v>
       </c>
@@ -60295,7 +60293,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>11</v>
       </c>
@@ -60330,7 +60328,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="176" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>11</v>
       </c>
@@ -60365,7 +60363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="177" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>11</v>
       </c>
@@ -60400,7 +60398,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="178" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>141</v>
       </c>
@@ -60435,7 +60433,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="179" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>11</v>
       </c>
@@ -60470,7 +60468,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="180" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>350</v>
       </c>
@@ -60505,7 +60503,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="181" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>11</v>
       </c>
@@ -60540,7 +60538,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="182" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>11</v>
       </c>
@@ -61546,7 +61544,7 @@
       <c r="AKS182"/>
       <c r="AKT182"/>
     </row>
-    <row r="183" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>11</v>
       </c>
@@ -61581,7 +61579,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="184" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>141</v>
       </c>
@@ -61616,7 +61614,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="185" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>11</v>
       </c>
@@ -62622,7 +62620,7 @@
       <c r="AKS185"/>
       <c r="AKT185"/>
     </row>
-    <row r="186" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>11</v>
       </c>
@@ -62657,7 +62655,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="187" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>11</v>
       </c>
@@ -63663,7 +63661,7 @@
       <c r="AKS187"/>
       <c r="AKT187"/>
     </row>
-    <row r="188" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>141</v>
       </c>
@@ -63698,7 +63696,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="189" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>350</v>
       </c>
@@ -63733,7 +63731,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="190" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>11</v>
       </c>
@@ -64739,7 +64737,7 @@
       <c r="AKS190"/>
       <c r="AKT190"/>
     </row>
-    <row r="191" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>11</v>
       </c>
@@ -65745,7 +65743,7 @@
       <c r="AKS191"/>
       <c r="AKT191"/>
     </row>
-    <row r="192" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>11</v>
       </c>
@@ -65780,7 +65778,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="193" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>11</v>
       </c>
@@ -65815,7 +65813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="194" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>11</v>
       </c>
@@ -65850,7 +65848,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="195" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>11</v>
       </c>
@@ -65885,7 +65883,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="196" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>350</v>
       </c>
@@ -65920,7 +65918,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="197" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>11</v>
       </c>
@@ -65955,7 +65953,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="198" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>350</v>
       </c>
@@ -66961,7 +66959,7 @@
       <c r="AKS198"/>
       <c r="AKT198"/>
     </row>
-    <row r="199" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>11</v>
       </c>
@@ -67967,7 +67965,7 @@
       <c r="AKS199"/>
       <c r="AKT199"/>
     </row>
-    <row r="200" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>11</v>
       </c>
@@ -68002,7 +68000,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="201" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>350</v>
       </c>
@@ -68037,7 +68035,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="202" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>11</v>
       </c>
@@ -68072,7 +68070,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="203" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>11</v>
       </c>
@@ -68107,7 +68105,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="204" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>11</v>
       </c>
@@ -69113,7 +69111,7 @@
       <c r="AKS204"/>
       <c r="AKT204"/>
     </row>
-    <row r="205" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>350</v>
       </c>
@@ -69148,7 +69146,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="206" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>350</v>
       </c>
@@ -69183,7 +69181,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="207" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>350</v>
       </c>
@@ -69218,7 +69216,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="208" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>11</v>
       </c>
@@ -69253,7 +69251,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="209" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>11</v>
       </c>
@@ -70259,7 +70257,7 @@
       <c r="AKS209"/>
       <c r="AKT209"/>
     </row>
-    <row r="210" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>11</v>
       </c>
@@ -70294,7 +70292,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="211" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>11</v>
       </c>
@@ -70329,7 +70327,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="212" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>11</v>
       </c>
@@ -71335,7 +71333,7 @@
       <c r="AKS212"/>
       <c r="AKT212"/>
     </row>
-    <row r="213" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>11</v>
       </c>
@@ -72341,7 +72339,7 @@
       <c r="AKS213"/>
       <c r="AKT213"/>
     </row>
-    <row r="214" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>350</v>
       </c>
@@ -72376,7 +72374,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="215" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>11</v>
       </c>
@@ -72411,7 +72409,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="216" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>11</v>
       </c>
@@ -72446,7 +72444,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="217" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>11</v>
       </c>
@@ -72481,7 +72479,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="218" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>141</v>
       </c>
@@ -72516,7 +72514,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="219" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>11</v>
       </c>
@@ -73522,7 +73520,7 @@
       <c r="AKS219"/>
       <c r="AKT219"/>
     </row>
-    <row r="220" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>11</v>
       </c>
@@ -73557,7 +73555,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="221" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>11</v>
       </c>
@@ -73592,7 +73590,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="222" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>141</v>
       </c>
@@ -73627,7 +73625,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="223" spans="1:982" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>90</v>
       </c>
@@ -73662,7 +73660,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="224" spans="1:982" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:982" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>350</v>
       </c>
@@ -75744,17 +75742,17 @@
         <v>378</v>
       </c>
     </row>
-    <row r="228" spans="1:982" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="6" t="s">
+    <row r="228" spans="1:982" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A228" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="B228" s="6" t="s">
+      <c r="B228" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="C228" s="6" t="s">
+      <c r="C228" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="D228" s="6" t="s">
+      <c r="D228" s="5" t="s">
         <v>377</v>
       </c>
       <c r="E228">
@@ -75766,30 +75764,30 @@
       <c r="G228">
         <v>0</v>
       </c>
-      <c r="H228" s="6">
+      <c r="H228" s="5">
         <v>20160</v>
       </c>
-      <c r="I228" s="6">
+      <c r="I228" s="5">
         <v>21499</v>
       </c>
-      <c r="J228" s="6">
+      <c r="J228" s="5">
         <v>1870</v>
       </c>
-      <c r="K228" s="6" t="s">
+      <c r="K228" s="5" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="229" spans="1:982" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="6" t="s">
+    <row r="229" spans="1:982" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="B229" s="6" t="s">
+      <c r="B229" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="C229" s="6" t="s">
+      <c r="C229" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="D229" s="6" t="s">
+      <c r="D229" s="5" t="s">
         <v>377</v>
       </c>
       <c r="E229">
@@ -75801,30 +75799,30 @@
       <c r="G229">
         <v>0</v>
       </c>
-      <c r="H229" s="6">
+      <c r="H229" s="5">
         <v>63000</v>
       </c>
-      <c r="I229" s="6">
+      <c r="I229" s="5">
         <v>65550</v>
       </c>
-      <c r="J229" s="6">
+      <c r="J229" s="5">
         <v>1355</v>
       </c>
-      <c r="K229" s="6" t="s">
+      <c r="K229" s="5" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="230" spans="1:982" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="6" t="s">
+    <row r="230" spans="1:982" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="B230" s="6" t="s">
+      <c r="B230" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="C230" s="6" t="s">
+      <c r="C230" s="5" t="s">
         <v>383</v>
       </c>
-      <c r="D230" s="6" t="s">
+      <c r="D230" s="5" t="s">
         <v>377</v>
       </c>
       <c r="E230">
@@ -75836,30 +75834,30 @@
       <c r="G230">
         <v>0</v>
       </c>
-      <c r="H230" s="6">
+      <c r="H230" s="5">
         <v>70000</v>
       </c>
-      <c r="I230" s="6">
+      <c r="I230" s="5">
         <v>71993</v>
       </c>
-      <c r="J230" s="6">
+      <c r="J230" s="5">
         <v>1399</v>
       </c>
-      <c r="K230" s="6" t="s">
+      <c r="K230" s="5" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="231" spans="1:982" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="6" t="s">
+    <row r="231" spans="1:982" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="B231" s="6" t="s">
+      <c r="B231" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="C231" s="6" t="s">
+      <c r="C231" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="D231" s="6" t="s">
+      <c r="D231" s="5" t="s">
         <v>377</v>
       </c>
       <c r="E231">
@@ -75871,30 +75869,30 @@
       <c r="G231">
         <v>0</v>
       </c>
-      <c r="H231" s="6">
+      <c r="H231" s="5">
         <v>56040</v>
       </c>
-      <c r="I231" s="6">
+      <c r="I231" s="5">
         <v>58982</v>
       </c>
-      <c r="J231" s="6">
+      <c r="J231" s="5">
         <v>2590</v>
       </c>
-      <c r="K231" s="6" t="s">
+      <c r="K231" s="5" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="232" spans="1:982" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="6" t="s">
+    <row r="232" spans="1:982" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="B232" s="6" t="s">
+      <c r="B232" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="C232" s="6" t="s">
+      <c r="C232" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="D232" s="6" t="s">
+      <c r="D232" s="5" t="s">
         <v>377</v>
       </c>
       <c r="E232">
@@ -75906,16 +75904,16 @@
       <c r="G232">
         <v>0</v>
       </c>
-      <c r="H232" s="6">
+      <c r="H232" s="5">
         <v>5200</v>
       </c>
-      <c r="I232" s="6">
+      <c r="I232" s="5">
         <v>5699</v>
       </c>
-      <c r="J232" s="6">
-        <v>0</v>
-      </c>
-      <c r="K232" s="6" t="s">
+      <c r="J232" s="5">
+        <v>0</v>
+      </c>
+      <c r="K232" s="5" t="s">
         <v>378</v>
       </c>
     </row>
@@ -75988,19 +75986,18 @@
       <c r="K234" t="s">
         <v>378</v>
       </c>
-      <c r="L234" s="5"/>
     </row>
-    <row r="235" spans="1:982" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="6" t="s">
+    <row r="235" spans="1:982" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="B235" s="6" t="s">
+      <c r="B235" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="C235" s="6" t="s">
+      <c r="C235" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="D235" s="6" t="s">
+      <c r="D235" s="5" t="s">
         <v>377</v>
       </c>
       <c r="E235">
@@ -76012,16 +76009,16 @@
       <c r="G235">
         <v>0</v>
       </c>
-      <c r="H235" s="6">
+      <c r="H235" s="5">
         <v>25000</v>
       </c>
-      <c r="I235" s="6">
+      <c r="I235" s="5">
         <v>27357</v>
       </c>
-      <c r="J235" s="6">
+      <c r="J235" s="5">
         <v>590</v>
       </c>
-      <c r="K235" s="6" t="s">
+      <c r="K235" s="5" t="s">
         <v>378</v>
       </c>
     </row>
@@ -76060,17 +76057,17 @@
         <v>378</v>
       </c>
     </row>
-    <row r="237" spans="1:982" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="6" t="s">
+    <row r="237" spans="1:982" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="B237" s="6" t="s">
+      <c r="B237" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="C237" s="6" t="s">
+      <c r="C237" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="D237" s="6" t="s">
+      <c r="D237" s="5" t="s">
         <v>377</v>
       </c>
       <c r="E237">
@@ -76082,16 +76079,16 @@
       <c r="G237">
         <v>0</v>
       </c>
-      <c r="H237" s="6">
+      <c r="H237" s="5">
         <v>9000</v>
       </c>
-      <c r="I237" s="6">
+      <c r="I237" s="5">
         <v>12072</v>
       </c>
-      <c r="J237" s="6">
+      <c r="J237" s="5">
         <v>138</v>
       </c>
-      <c r="K237" s="6" t="s">
+      <c r="K237" s="5" t="s">
         <v>378</v>
       </c>
     </row>
@@ -76164,7 +76161,6 @@
       <c r="K239" t="s">
         <v>378</v>
       </c>
-      <c r="L239" s="5"/>
     </row>
     <row r="240" spans="1:982" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
@@ -76201,17 +76197,17 @@
         <v>378</v>
       </c>
     </row>
-    <row r="241" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="6" t="s">
+    <row r="241" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="B241" s="6" t="s">
+      <c r="B241" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="C241" s="6" t="s">
+      <c r="C241" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="D241" s="6" t="s">
+      <c r="D241" s="5" t="s">
         <v>377</v>
       </c>
       <c r="E241">
@@ -76223,30 +76219,30 @@
       <c r="G241">
         <v>0</v>
       </c>
-      <c r="H241" s="6">
+      <c r="H241" s="5">
         <v>25139.3</v>
       </c>
-      <c r="I241" s="6">
+      <c r="I241" s="5">
         <v>25390.09</v>
       </c>
-      <c r="J241" s="6">
+      <c r="J241" s="5">
         <v>2910.31</v>
       </c>
-      <c r="K241" s="6" t="s">
+      <c r="K241" s="5" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="242" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A242" s="6" t="s">
+    <row r="242" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="B242" s="6" t="s">
+      <c r="B242" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="C242" s="6" t="s">
+      <c r="C242" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="D242" s="6" t="s">
+      <c r="D242" s="5" t="s">
         <v>377</v>
       </c>
       <c r="E242">
@@ -76258,21 +76254,21 @@
       <c r="G242">
         <v>0</v>
       </c>
-      <c r="H242" s="6">
+      <c r="H242" s="5">
         <v>22000</v>
       </c>
-      <c r="I242" s="6">
+      <c r="I242" s="5">
         <v>23410</v>
       </c>
-      <c r="J242" s="6">
+      <c r="J242" s="5">
         <v>265</v>
       </c>
-      <c r="K242" s="6" t="s">
+      <c r="K242" s="5" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="243" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A243" s="5" t="s">
+      <c r="A243" t="s">
         <v>374</v>
       </c>
       <c r="B243" t="s">
@@ -76306,17 +76302,17 @@
         <v>378</v>
       </c>
     </row>
-    <row r="244" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A244" s="6" t="s">
+    <row r="244" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="B244" s="6" t="s">
+      <c r="B244" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="C244" s="6" t="s">
+      <c r="C244" s="5" t="s">
         <v>397</v>
       </c>
-      <c r="D244" s="6" t="s">
+      <c r="D244" s="5" t="s">
         <v>377</v>
       </c>
       <c r="E244">
@@ -76328,16 +76324,16 @@
       <c r="G244">
         <v>0</v>
       </c>
-      <c r="H244" s="6">
+      <c r="H244" s="5">
         <v>21000</v>
       </c>
-      <c r="I244" s="6">
+      <c r="I244" s="5">
         <v>23410</v>
       </c>
-      <c r="J244" s="6">
+      <c r="J244" s="5">
         <v>744</v>
       </c>
-      <c r="K244" s="6" t="s">
+      <c r="K244" s="5" t="s">
         <v>378</v>
       </c>
     </row>
@@ -76376,17 +76372,17 @@
         <v>378</v>
       </c>
     </row>
-    <row r="246" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A246" s="6" t="s">
+    <row r="246" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="B246" s="6" t="s">
+      <c r="B246" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="C246" s="6" t="s">
+      <c r="C246" s="5" t="s">
         <v>399</v>
       </c>
-      <c r="D246" s="6" t="s">
+      <c r="D246" s="5" t="s">
         <v>377</v>
       </c>
       <c r="E246">
@@ -76398,30 +76394,30 @@
       <c r="G246">
         <v>0</v>
       </c>
-      <c r="H246" s="6">
+      <c r="H246" s="5">
         <v>96530</v>
       </c>
-      <c r="I246" s="6">
+      <c r="I246" s="5">
         <v>99090</v>
       </c>
-      <c r="J246" s="6">
+      <c r="J246" s="5">
         <v>2939</v>
       </c>
-      <c r="K246" s="6" t="s">
+      <c r="K246" s="5" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="247" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A247" s="6" t="s">
+    <row r="247" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="B247" s="6" t="s">
+      <c r="B247" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="C247" s="6" t="s">
+      <c r="C247" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="D247" s="6" t="s">
+      <c r="D247" s="5" t="s">
         <v>377</v>
       </c>
       <c r="E247">
@@ -76433,16 +76429,16 @@
       <c r="G247">
         <v>0</v>
       </c>
-      <c r="H247" s="6">
+      <c r="H247" s="5">
         <v>8000</v>
       </c>
-      <c r="I247" s="6">
+      <c r="I247" s="5">
         <v>8871</v>
       </c>
-      <c r="J247" s="6">
+      <c r="J247" s="5">
         <v>754</v>
       </c>
-      <c r="K247" s="6" t="s">
+      <c r="K247" s="5" t="s">
         <v>378</v>
       </c>
     </row>
@@ -76516,17 +76512,17 @@
         <v>378</v>
       </c>
     </row>
-    <row r="250" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A250" s="6" t="s">
+    <row r="250" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A250" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="B250" s="6" t="s">
+      <c r="B250" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="C250" s="6" t="s">
+      <c r="C250" s="5" t="s">
         <v>403</v>
       </c>
-      <c r="D250" s="6" t="s">
+      <c r="D250" s="5" t="s">
         <v>377</v>
       </c>
       <c r="E250">
@@ -76538,16 +76534,16 @@
       <c r="G250">
         <v>0</v>
       </c>
-      <c r="H250" s="6">
+      <c r="H250" s="5">
         <v>8800</v>
       </c>
-      <c r="I250" s="6">
+      <c r="I250" s="5">
         <v>8900</v>
       </c>
-      <c r="J250" s="6">
+      <c r="J250" s="5">
         <v>295</v>
       </c>
-      <c r="K250" s="6" t="s">
+      <c r="K250" s="5" t="s">
         <v>378</v>
       </c>
     </row>
@@ -76586,17 +76582,17 @@
         <v>378</v>
       </c>
     </row>
-    <row r="252" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A252" s="6" t="s">
+    <row r="252" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A252" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="B252" s="6" t="s">
+      <c r="B252" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="C252" s="6" t="s">
+      <c r="C252" s="5" t="s">
         <v>405</v>
       </c>
-      <c r="D252" s="6" t="s">
+      <c r="D252" s="5" t="s">
         <v>377</v>
       </c>
       <c r="E252">
@@ -76608,16 +76604,16 @@
       <c r="G252">
         <v>0</v>
       </c>
-      <c r="H252" s="6">
+      <c r="H252" s="5">
         <v>10000</v>
       </c>
-      <c r="I252" s="6">
+      <c r="I252" s="5">
         <v>10148</v>
       </c>
-      <c r="J252" s="6">
+      <c r="J252" s="5">
         <v>2922</v>
       </c>
-      <c r="K252" s="6" t="s">
+      <c r="K252" s="5" t="s">
         <v>378</v>
       </c>
     </row>
@@ -76656,7 +76652,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="254" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>350</v>
       </c>
@@ -76691,7 +76687,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="255" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>11</v>
       </c>
@@ -76726,7 +76722,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="256" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>350</v>
       </c>
@@ -76761,7 +76757,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="257" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>90</v>
       </c>
@@ -76796,7 +76792,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="258" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>11</v>
       </c>
@@ -76831,7 +76827,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="259" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>11</v>
       </c>
@@ -76866,7 +76862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="260" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>11</v>
       </c>
@@ -76901,7 +76897,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="261" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>141</v>
       </c>
@@ -76936,7 +76932,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="262" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>141</v>
       </c>
@@ -76971,7 +76967,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="263" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>141</v>
       </c>
@@ -77006,7 +77002,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="264" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>141</v>
       </c>
@@ -77041,7 +77037,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="265" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>141</v>
       </c>
@@ -77076,7 +77072,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="266" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>141</v>
       </c>
@@ -77111,7 +77107,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="267" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>141</v>
       </c>
@@ -77146,7 +77142,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="268" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>141</v>
       </c>
@@ -77181,7 +77177,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="269" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>141</v>
       </c>
@@ -77216,7 +77212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="270" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>141</v>
       </c>
@@ -77251,7 +77247,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="271" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>141</v>
       </c>
@@ -77286,7 +77282,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="272" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>141</v>
       </c>
@@ -77321,7 +77317,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="273" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>141</v>
       </c>
@@ -77356,7 +77352,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="274" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>141</v>
       </c>
@@ -77391,7 +77387,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="275" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>141</v>
       </c>
@@ -77426,7 +77422,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="276" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>141</v>
       </c>
@@ -77461,7 +77457,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="277" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>141</v>
       </c>
@@ -77496,7 +77492,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="278" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>141</v>
       </c>
@@ -77531,7 +77527,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="279" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
         <v>141</v>
       </c>
@@ -77566,7 +77562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="280" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
         <v>141</v>
       </c>
@@ -77601,7 +77597,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="281" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
         <v>141</v>
       </c>
@@ -77636,7 +77632,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="282" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
         <v>141</v>
       </c>
@@ -77671,7 +77667,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="283" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>141</v>
       </c>
@@ -77706,7 +77702,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="284" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
         <v>141</v>
       </c>
@@ -77741,7 +77737,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="285" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
         <v>141</v>
       </c>
@@ -77776,7 +77772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="286" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
         <v>141</v>
       </c>
@@ -77811,7 +77807,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="287" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
         <v>141</v>
       </c>
@@ -77846,7 +77842,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="288" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>141</v>
       </c>
@@ -77881,7 +77877,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="289" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
         <v>141</v>
       </c>
@@ -77916,7 +77912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="290" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
         <v>141</v>
       </c>
@@ -77951,7 +77947,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="291" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
         <v>141</v>
       </c>
@@ -77986,7 +77982,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="292" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
         <v>141</v>
       </c>
@@ -78021,7 +78017,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="293" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
         <v>141</v>
       </c>
@@ -78056,7 +78052,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="294" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
         <v>141</v>
       </c>
@@ -78091,7 +78087,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="295" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
         <v>141</v>
       </c>
@@ -78126,7 +78122,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="296" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
         <v>141</v>
       </c>
@@ -78161,7 +78157,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="297" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
         <v>141</v>
       </c>
@@ -78196,7 +78192,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="298" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
         <v>141</v>
       </c>
@@ -78231,7 +78227,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="299" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
         <v>141</v>
       </c>
@@ -78266,7 +78262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="300" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
         <v>141</v>
       </c>
@@ -78303,11 +78299,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K300" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="BUNKER - (-)"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K300">
       <sortCondition descending="1" ref="G1:G300"/>
     </sortState>

</xml_diff>